<commit_message>
richards: piecewiselinear sink docoed and tested, at least for singlephase
r25022
</commit_message>
<xml_diff>
--- a/modules/combined/doc/richards/tests/data/sinks.xlsx
+++ b/modules/combined/doc/richards/tests/data/sinks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="108" windowWidth="15300" windowHeight="11112" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="108" windowWidth="15300" windowHeight="11112" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="piecewise_linear_chart" sheetId="4" r:id="rId1"/>
@@ -6261,7 +6261,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -13751,8 +13751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:R204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" activeCellId="1" sqref="I5:I41 M5:M41"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>